<commit_message>
Updated counterbalance sheet and added script for experiment 2.
</commit_message>
<xml_diff>
--- a/counterbalance.xlsx
+++ b/counterbalance.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilyhembacher/Desktop/soc_ref_uncert/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23913"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="6640" yWindow="1420" windowWidth="14940" windowHeight="11780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="52">
   <si>
     <t>Novel 1</t>
   </si>
@@ -102,13 +97,94 @@
   </si>
   <si>
     <t>Condition</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>F1 F2</t>
+  </si>
+  <si>
+    <t>N1 N2</t>
+  </si>
+  <si>
+    <t>F2 F3</t>
+  </si>
+  <si>
+    <t>N2 N3</t>
+  </si>
+  <si>
+    <t>F3 N3</t>
+  </si>
+  <si>
+    <t>F4 N4</t>
+  </si>
+  <si>
+    <t>F4 F5</t>
+  </si>
+  <si>
+    <t>N4 N5</t>
+  </si>
+  <si>
+    <t>F6 N6</t>
+  </si>
+  <si>
+    <t>F7 F8</t>
+  </si>
+  <si>
+    <t>N7 N8</t>
+  </si>
+  <si>
+    <t>F9 N9</t>
+  </si>
+  <si>
+    <t>F10 F11</t>
+  </si>
+  <si>
+    <t>N10 N11</t>
+  </si>
+  <si>
+    <t>F12 N12</t>
+  </si>
+  <si>
+    <t>F5 F6</t>
+  </si>
+  <si>
+    <t>N5 N6</t>
+  </si>
+  <si>
+    <t>F7 N7</t>
+  </si>
+  <si>
+    <t>F8 F9</t>
+  </si>
+  <si>
+    <t>N8 N9</t>
+  </si>
+  <si>
+    <t>F10 N10</t>
+  </si>
+  <si>
+    <t>F11 F12</t>
+  </si>
+  <si>
+    <t>N11 N12</t>
+  </si>
+  <si>
+    <t>F1 N1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,6 +208,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -150,17 +234,82 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -216,7 +365,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -251,7 +400,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -428,7 +577,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -436,23 +585,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="E20" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="24.1640625" customWidth="1"/>
     <col min="3" max="3" width="21.83203125" customWidth="1"/>
     <col min="4" max="4" width="25.1640625" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="8" max="9" width="20.5" customWidth="1"/>
-    <col min="10" max="11" width="20.1640625" customWidth="1"/>
+    <col min="5" max="7" width="24.33203125" customWidth="1"/>
+    <col min="10" max="11" width="20.5" customWidth="1"/>
+    <col min="12" max="13" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -469,7 +618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -483,7 +632,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -497,7 +646,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -511,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -525,7 +674,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -539,7 +688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -553,7 +702,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -567,7 +716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -581,7 +730,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -595,7 +744,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="B11" t="s">
         <v>16</v>
       </c>
@@ -609,7 +758,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -623,7 +772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="B13" t="s">
         <v>17</v>
       </c>
@@ -637,8 +786,361 @@
         <v>23</v>
       </c>
     </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" t="s">
+        <v>43</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" t="s">
+        <v>36</v>
+      </c>
+      <c r="J31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" t="s">
+        <v>37</v>
+      </c>
+      <c r="J32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" t="s">
+        <v>46</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I33" t="s">
+        <v>38</v>
+      </c>
+      <c r="J33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" t="s">
+        <v>47</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F35" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" t="s">
+        <v>48</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" t="s">
+        <v>40</v>
+      </c>
+      <c r="J35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F36" t="s">
+        <v>40</v>
+      </c>
+      <c r="G36" t="s">
+        <v>49</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I36" t="s">
+        <v>41</v>
+      </c>
+      <c r="J36" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" t="s">
+        <v>41</v>
+      </c>
+      <c r="G37" t="s">
+        <v>50</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I37" t="s">
+        <v>42</v>
+      </c>
+      <c r="J37" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" t="s">
+        <v>51</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I39" t="s">
+        <v>29</v>
+      </c>
+      <c r="J39" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>